<commit_message>
Forgotten commit with updated excel files for double-antigentest stuff
</commit_message>
<xml_diff>
--- a/Interactive/HurtigTests/dobbelt_test.xlsx
+++ b/Interactive/HurtigTests/dobbelt_test.xlsx
@@ -386,6 +386,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -395,23 +412,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,8 +695,8 @@
   <dimension ref="A1:Q105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I97" sqref="I97"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -719,22 +719,22 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="40" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="5"/>
@@ -754,12 +754,12 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="2"/>
     </row>
@@ -777,12 +777,12 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
       <c r="P3" s="9"/>
       <c r="Q3" s="3"/>
     </row>
@@ -838,64 +838,64 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="40">
+      <c r="A5" s="34">
         <v>0</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5" s="35">
         <f t="shared" ref="B5:B36" si="0">A5*B$1+(1-A5)*(1-B$2)</f>
         <v>5.0000000000000044E-3</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="35">
         <f t="shared" ref="C5:C36" si="1">A5*B$1/B5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="35">
         <f t="shared" ref="D5:D36" si="2">$A5*$B$1*$B$1+(1-$A5)*(1-$B$2)*(1-$B$2)</f>
         <v>2.5000000000000045E-5</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="35">
         <f t="shared" ref="E5:E36" si="3">A5*B$1*B$1/D5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="41">
+      <c r="F5" s="35">
         <f t="shared" ref="F5:F36" si="4">$A5*$B$1*(1-$B$1)+(1-$A5)*$B$2*(1-$B$2)</f>
         <v>4.9750000000000046E-3</v>
       </c>
-      <c r="G5" s="41">
+      <c r="G5" s="35">
         <f t="shared" ref="G5:G36" si="5">A5*B$1*(1-B$1)/F5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43">
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="37">
         <f t="shared" ref="J5:J36" si="6">$B$3*B5</f>
         <v>500.00000000000045</v>
       </c>
-      <c r="K5" s="43">
+      <c r="K5" s="37">
         <f t="shared" ref="K5:K36" si="7">$B$3*D5</f>
         <v>2.5000000000000044</v>
       </c>
-      <c r="L5" s="43">
+      <c r="L5" s="37">
         <f t="shared" ref="L5:L36" si="8">K5*E5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="43">
+      <c r="M5" s="37">
         <f t="shared" ref="M5:M36" si="9">K5-L5</f>
         <v>2.5000000000000044</v>
       </c>
-      <c r="N5" s="43">
+      <c r="N5" s="37">
         <f t="shared" ref="N5:N36" si="10">F5*$B$3</f>
         <v>497.50000000000045</v>
       </c>
-      <c r="O5" s="43">
+      <c r="O5" s="37">
         <f t="shared" ref="O5:O36" si="11">N5*G5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="44">
+      <c r="P5" s="38">
         <f>(J5-K5-O5)/J5</f>
         <v>0.995</v>
       </c>
-      <c r="Q5" s="45"/>
+      <c r="Q5" s="39"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
@@ -954,7 +954,7 @@
         <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
-      <c r="P6" s="38">
+      <c r="P6" s="32">
         <f t="shared" ref="P6:P69" si="13">(J6-K6-O6)/J6</f>
         <v>0.98514753936033272</v>
       </c>
@@ -1021,7 +1021,7 @@
         <f t="shared" si="11"/>
         <v>5.0000000000000009</v>
       </c>
-      <c r="P7" s="38">
+      <c r="P7" s="32">
         <f t="shared" si="13"/>
         <v>0.97548636987644632</v>
       </c>
@@ -1088,7 +1088,7 @@
         <f t="shared" si="11"/>
         <v>7.5000000000000009</v>
       </c>
-      <c r="P8" s="38">
+      <c r="P8" s="32">
         <f t="shared" si="13"/>
         <v>0.96601097407011749</v>
       </c>
@@ -1155,7 +1155,7 @@
         <f t="shared" si="11"/>
         <v>10.000000000000002</v>
       </c>
-      <c r="P9" s="38">
+      <c r="P9" s="32">
         <f t="shared" si="13"/>
         <v>0.956716044632551</v>
       </c>
@@ -1222,7 +1222,7 @@
         <f t="shared" si="11"/>
         <v>12.5</v>
       </c>
-      <c r="P10" s="38">
+      <c r="P10" s="32">
         <f t="shared" si="13"/>
         <v>0.94759647451167217</v>
       </c>
@@ -1289,7 +1289,7 @@
         <f t="shared" si="11"/>
         <v>15</v>
       </c>
-      <c r="P11" s="38">
+      <c r="P11" s="32">
         <f t="shared" si="13"/>
         <v>0.93864734755521995</v>
       </c>
@@ -1356,7 +1356,7 @@
         <f t="shared" si="11"/>
         <v>17.5</v>
       </c>
-      <c r="P12" s="38">
+      <c r="P12" s="32">
         <f t="shared" si="13"/>
         <v>0.92986392967361831</v>
       </c>
@@ -1423,7 +1423,7 @@
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
-      <c r="P13" s="38">
+      <c r="P13" s="32">
         <f t="shared" si="13"/>
         <v>0.92124166048925127</v>
       </c>
@@ -1490,7 +1490,7 @@
         <f t="shared" si="11"/>
         <v>22.500000000000007</v>
       </c>
-      <c r="P14" s="38">
+      <c r="P14" s="32">
         <f t="shared" si="13"/>
         <v>0.91277614544119001</v>
       </c>
@@ -1557,7 +1557,7 @@
         <f t="shared" si="11"/>
         <v>25.000000000000007</v>
       </c>
-      <c r="P15" s="38">
+      <c r="P15" s="32">
         <f t="shared" si="13"/>
         <v>0.90446314831665142</v>
       </c>
@@ -1624,7 +1624,7 @@
         <f t="shared" si="11"/>
         <v>27.500000000000011</v>
       </c>
-      <c r="P16" s="38">
+      <c r="P16" s="32">
         <f t="shared" si="13"/>
         <v>0.89629858418252328</v>
       </c>
@@ -1691,7 +1691,7 @@
         <f t="shared" si="11"/>
         <v>30.000000000000011</v>
       </c>
-      <c r="P17" s="38">
+      <c r="P17" s="32">
         <f t="shared" si="13"/>
         <v>0.8882785126921704</v>
       </c>
@@ -1758,7 +1758,7 @@
         <f t="shared" si="11"/>
         <v>32.500000000000014</v>
       </c>
-      <c r="P18" s="38">
+      <c r="P18" s="32">
         <f t="shared" si="13"/>
         <v>0.88039913174448492</v>
       </c>
@@ -1825,7 +1825,7 @@
         <f t="shared" si="11"/>
         <v>35.000000000000014</v>
       </c>
-      <c r="P19" s="38">
+      <c r="P19" s="32">
         <f t="shared" si="13"/>
         <v>0.87265677147373988</v>
       </c>
@@ -1892,7 +1892,7 @@
         <f t="shared" si="11"/>
         <v>37.500000000000007</v>
       </c>
-      <c r="P20" s="38">
+      <c r="P20" s="32">
         <f t="shared" si="13"/>
         <v>0.86504788855028303</v>
       </c>
@@ -1959,7 +1959,7 @@
         <f t="shared" si="11"/>
         <v>40.000000000000014</v>
       </c>
-      <c r="P21" s="38">
+      <c r="P21" s="32">
         <f t="shared" si="13"/>
         <v>0.85756906077348083</v>
       </c>
@@ -2026,7 +2026,7 @@
         <f t="shared" si="11"/>
         <v>42.500000000000007</v>
       </c>
-      <c r="P22" s="38">
+      <c r="P22" s="32">
         <f t="shared" si="13"/>
         <v>0.8502169819395704</v>
       </c>
@@ -2093,7 +2093,7 @@
         <f t="shared" si="11"/>
         <v>45.000000000000014</v>
       </c>
-      <c r="P23" s="38">
+      <c r="P23" s="32">
         <f t="shared" si="13"/>
         <v>0.84298845696825675</v>
       </c>
@@ -2160,7 +2160,7 @@
         <f t="shared" si="11"/>
         <v>47.500000000000014</v>
       </c>
-      <c r="P24" s="38">
+      <c r="P24" s="32">
         <f t="shared" si="13"/>
         <v>0.83588039727295682</v>
       </c>
@@ -2227,7 +2227,7 @@
         <f t="shared" si="11"/>
         <v>50.000000000000014</v>
       </c>
-      <c r="P25" s="38">
+      <c r="P25" s="32">
         <f t="shared" si="13"/>
         <v>0.82888981636060111</v>
       </c>
@@ -2294,7 +2294,7 @@
         <f t="shared" si="11"/>
         <v>52.500000000000007</v>
       </c>
-      <c r="P26" s="38">
+      <c r="P26" s="32">
         <f t="shared" si="13"/>
         <v>0.82201382564781855</v>
       </c>
@@ -2361,7 +2361,7 @@
         <f t="shared" si="11"/>
         <v>54.999999999999993</v>
       </c>
-      <c r="P27" s="38">
+      <c r="P27" s="32">
         <f t="shared" si="13"/>
         <v>0.8152496304811957</v>
       </c>
@@ -2428,7 +2428,7 @@
         <f t="shared" si="11"/>
         <v>57.499999999999993</v>
       </c>
-      <c r="P28" s="38">
+      <c r="P28" s="32">
         <f t="shared" si="13"/>
         <v>0.80859452635008566</v>
       </c>
@@ -2495,7 +2495,7 @@
         <f t="shared" si="11"/>
         <v>59.999999999999993</v>
       </c>
-      <c r="P29" s="38">
+      <c r="P29" s="32">
         <f t="shared" si="13"/>
         <v>0.80204589528118952</v>
       </c>
@@ -2562,7 +2562,7 @@
         <f t="shared" si="11"/>
         <v>62.499999999999986</v>
       </c>
-      <c r="P30" s="38">
+      <c r="P30" s="32">
         <f t="shared" si="13"/>
         <v>0.7956012024048098</v>
       </c>
@@ -2629,7 +2629,7 @@
         <f t="shared" si="11"/>
         <v>64.999999999999986</v>
       </c>
-      <c r="P31" s="38">
+      <c r="P31" s="32">
         <f t="shared" si="13"/>
         <v>0.78925799268331498</v>
       </c>
@@ -2696,7 +2696,7 @@
         <f t="shared" si="11"/>
         <v>67.499999999999972</v>
       </c>
-      <c r="P32" s="38">
+      <c r="P32" s="32">
         <f t="shared" si="13"/>
         <v>0.78301388779294578</v>
       </c>
@@ -2763,7 +2763,7 @@
         <f t="shared" si="11"/>
         <v>69.999999999999986</v>
       </c>
-      <c r="P33" s="38">
+      <c r="P33" s="32">
         <f t="shared" si="13"/>
         <v>0.77686658315064228</v>
       </c>
@@ -2830,7 +2830,7 @@
         <f t="shared" si="11"/>
         <v>72.499999999999986</v>
       </c>
-      <c r="P34" s="38">
+      <c r="P34" s="32">
         <f t="shared" si="13"/>
         <v>0.7708138450780827</v>
       </c>
@@ -2897,7 +2897,7 @@
         <f t="shared" si="11"/>
         <v>74.999999999999972</v>
       </c>
-      <c r="P35" s="38">
+      <c r="P35" s="32">
         <f t="shared" si="13"/>
         <v>0.76485350809560548</v>
       </c>
@@ -2964,7 +2964,7 @@
         <f t="shared" si="11"/>
         <v>77.499999999999972</v>
       </c>
-      <c r="P36" s="38">
+      <c r="P36" s="32">
         <f t="shared" si="13"/>
         <v>0.75898347233912322</v>
       </c>
@@ -3031,7 +3031,7 @@
         <f t="shared" ref="O37:O68" si="27">N37*G37</f>
         <v>79.999999999999957</v>
       </c>
-      <c r="P37" s="38">
+      <c r="P37" s="32">
         <f t="shared" si="13"/>
         <v>0.75320170109356044</v>
       </c>
@@ -3098,7 +3098,7 @@
         <f t="shared" si="27"/>
         <v>82.499999999999943</v>
       </c>
-      <c r="P38" s="38">
+      <c r="P38" s="32">
         <f t="shared" si="13"/>
         <v>0.74750621843672305</v>
       </c>
@@ -3165,7 +3165,7 @@
         <f t="shared" si="27"/>
         <v>84.999999999999943</v>
       </c>
-      <c r="P39" s="38">
+      <c r="P39" s="32">
         <f t="shared" si="13"/>
         <v>0.74189510698787997</v>
       </c>
@@ -3232,7 +3232,7 @@
         <f t="shared" si="27"/>
         <v>87.499999999999943</v>
       </c>
-      <c r="P40" s="38">
+      <c r="P40" s="32">
         <f t="shared" si="13"/>
         <v>0.7363665057556632</v>
       </c>
@@ -3299,7 +3299,7 @@
         <f t="shared" si="27"/>
         <v>89.999999999999943</v>
       </c>
-      <c r="P41" s="38">
+      <c r="P41" s="32">
         <f t="shared" si="13"/>
         <v>0.73091860808021258</v>
       </c>
@@ -3366,7 +3366,7 @@
         <f t="shared" si="27"/>
         <v>92.499999999999943</v>
       </c>
-      <c r="P42" s="38">
+      <c r="P42" s="32">
         <f t="shared" si="13"/>
         <v>0.72554965966478835</v>
       </c>
@@ -3433,7 +3433,7 @@
         <f t="shared" si="27"/>
         <v>94.999999999999943</v>
       </c>
-      <c r="P43" s="38">
+      <c r="P43" s="32">
         <f t="shared" si="13"/>
         <v>0.72025795669234161</v>
       </c>
@@ -3500,7 +3500,7 @@
         <f t="shared" si="27"/>
         <v>97.499999999999929</v>
       </c>
-      <c r="P44" s="38">
+      <c r="P44" s="32">
         <f t="shared" si="13"/>
         <v>0.71504184402279802</v>
       </c>
@@ -3567,7 +3567,7 @@
         <f t="shared" si="27"/>
         <v>99.999999999999943</v>
       </c>
-      <c r="P45" s="38">
+      <c r="P45" s="32">
         <f t="shared" si="13"/>
         <v>0.70989971346704905</v>
       </c>
@@ -3634,7 +3634,7 @@
         <f t="shared" si="27"/>
         <v>102.49999999999996</v>
       </c>
-      <c r="P46" s="38">
+      <c r="P46" s="32">
         <f t="shared" si="13"/>
         <v>0.70483000213386471</v>
       </c>
@@ -3701,7 +3701,7 @@
         <f t="shared" si="27"/>
         <v>104.99999999999996</v>
       </c>
-      <c r="P47" s="38">
+      <c r="P47" s="32">
         <f t="shared" si="13"/>
         <v>0.69983119084616507</v>
       </c>
@@ -3768,7 +3768,7 @@
         <f t="shared" si="27"/>
         <v>107.49999999999996</v>
       </c>
-      <c r="P48" s="38">
+      <c r="P48" s="32">
         <f t="shared" si="13"/>
         <v>0.69490180262327306</v>
       </c>
@@ -3835,7 +3835,7 @@
         <f t="shared" si="27"/>
         <v>109.99999999999996</v>
       </c>
-      <c r="P49" s="38">
+      <c r="P49" s="32">
         <f t="shared" si="13"/>
         <v>0.69004040122596844</v>
       </c>
@@ -3902,7 +3902,7 @@
         <f t="shared" si="27"/>
         <v>112.49999999999999</v>
       </c>
-      <c r="P50" s="38">
+      <c r="P50" s="32">
         <f t="shared" si="13"/>
         <v>0.68524558976132843</v>
       </c>
@@ -3969,7 +3969,7 @@
         <f t="shared" si="27"/>
         <v>114.99999999999999</v>
       </c>
-      <c r="P51" s="38">
+      <c r="P51" s="32">
         <f t="shared" si="13"/>
         <v>0.68051600934451018</v>
       </c>
@@ -4036,7 +4036,7 @@
         <f t="shared" si="27"/>
         <v>117.5</v>
       </c>
-      <c r="P52" s="38">
+      <c r="P52" s="32">
         <f t="shared" si="13"/>
         <v>0.67585033781478221</v>
       </c>
@@ -4103,7 +4103,7 @@
         <f t="shared" si="27"/>
         <v>120</v>
       </c>
-      <c r="P53" s="38">
+      <c r="P53" s="32">
         <f t="shared" si="13"/>
         <v>0.67124728850325388</v>
       </c>
@@ -4170,7 +4170,7 @@
         <f t="shared" si="27"/>
         <v>122.50000000000001</v>
       </c>
-      <c r="P54" s="38">
+      <c r="P54" s="32">
         <f t="shared" si="13"/>
         <v>0.66670560904989584</v>
       </c>
@@ -4237,7 +4237,7 @@
         <f t="shared" si="27"/>
         <v>125</v>
       </c>
-      <c r="P55" s="38">
+      <c r="P55" s="32">
         <f t="shared" si="13"/>
         <v>0.66222408026755875</v>
       </c>
@@ -4304,7 +4304,7 @@
         <f t="shared" si="27"/>
         <v>127.50000000000001</v>
       </c>
-      <c r="P56" s="38">
+      <c r="P56" s="32">
         <f t="shared" si="13"/>
         <v>0.65780151505083406</v>
       </c>
@@ -4371,7 +4371,7 @@
         <f t="shared" si="27"/>
         <v>130.00000000000003</v>
       </c>
-      <c r="P57" s="38">
+      <c r="P57" s="32">
         <f t="shared" si="13"/>
         <v>0.65343675732770024</v>
       </c>
@@ -4438,7 +4438,7 @@
         <f t="shared" si="27"/>
         <v>132.50000000000003</v>
       </c>
-      <c r="P58" s="38">
+      <c r="P58" s="32">
         <f t="shared" si="13"/>
         <v>0.64912868105201038</v>
       </c>
@@ -4505,7 +4505,7 @@
         <f t="shared" si="27"/>
         <v>135.00000000000003</v>
       </c>
-      <c r="P59" s="38">
+      <c r="P59" s="32">
         <f t="shared" si="13"/>
         <v>0.64487618923498002</v>
       </c>
@@ -4572,7 +4572,7 @@
         <f t="shared" si="27"/>
         <v>137.50000000000003</v>
       </c>
-      <c r="P60" s="38">
+      <c r="P60" s="32">
         <f t="shared" si="13"/>
         <v>0.64067821301392058</v>
       </c>
@@ -4639,7 +4639,7 @@
         <f t="shared" si="27"/>
         <v>140.00000000000006</v>
       </c>
-      <c r="P61" s="38">
+      <c r="P61" s="32">
         <f t="shared" si="13"/>
         <v>0.63653371075656207</v>
       </c>
@@ -4706,7 +4706,7 @@
         <f t="shared" si="27"/>
         <v>142.50000000000006</v>
       </c>
-      <c r="P62" s="38">
+      <c r="P62" s="32">
         <f t="shared" si="13"/>
         <v>0.63244166719938644</v>
       </c>
@@ -4773,7 +4773,7 @@
         <f t="shared" si="27"/>
         <v>145.00000000000006</v>
       </c>
-      <c r="P63" s="38">
+      <c r="P63" s="32">
         <f t="shared" si="13"/>
         <v>0.62840109261847288</v>
       </c>
@@ -4840,7 +4840,7 @@
         <f t="shared" si="27"/>
         <v>147.50000000000006</v>
       </c>
-      <c r="P64" s="38">
+      <c r="P64" s="32">
         <f t="shared" si="13"/>
         <v>0.6244110220314375</v>
       </c>
@@ -4907,7 +4907,7 @@
         <f t="shared" si="27"/>
         <v>150.00000000000006</v>
       </c>
-      <c r="P65" s="38">
+      <c r="P65" s="32">
         <f t="shared" si="13"/>
         <v>0.62047051442910928</v>
       </c>
@@ -4974,7 +4974,7 @@
         <f t="shared" si="27"/>
         <v>152.50000000000009</v>
       </c>
-      <c r="P66" s="38">
+      <c r="P66" s="32">
         <f t="shared" si="13"/>
         <v>0.61657865203566309</v>
       </c>
@@ -5041,7 +5041,7 @@
         <f t="shared" si="27"/>
         <v>155.00000000000009</v>
       </c>
-      <c r="P67" s="38">
+      <c r="P67" s="32">
         <f t="shared" si="13"/>
         <v>0.61273453959598467</v>
       </c>
@@ -5108,7 +5108,7 @@
         <f t="shared" si="27"/>
         <v>157.50000000000009</v>
       </c>
-      <c r="P68" s="38">
+      <c r="P68" s="32">
         <f t="shared" si="13"/>
         <v>0.60893730368910515</v>
       </c>
@@ -5175,7 +5175,7 @@
         <f t="shared" ref="O69:O100" si="42">N69*G69</f>
         <v>160.00000000000009</v>
       </c>
-      <c r="P69" s="38">
+      <c r="P69" s="32">
         <f t="shared" si="13"/>
         <v>0.60518609206660134</v>
       </c>
@@ -5242,7 +5242,7 @@
         <f t="shared" si="42"/>
         <v>162.50000000000009</v>
       </c>
-      <c r="P70" s="38">
+      <c r="P70" s="32">
         <f t="shared" ref="P70:P105" si="44">(J70-K70-O70)/J70</f>
         <v>0.60148007301490725</v>
       </c>
@@ -5309,7 +5309,7 @@
         <f t="shared" si="42"/>
         <v>165.00000000000009</v>
       </c>
-      <c r="P71" s="38">
+      <c r="P71" s="32">
         <f t="shared" si="44"/>
         <v>0.59781843474053487</v>
       </c>
@@ -5376,7 +5376,7 @@
         <f t="shared" si="42"/>
         <v>167.50000000000014</v>
       </c>
-      <c r="P72" s="38">
+      <c r="P72" s="32">
         <f t="shared" si="44"/>
         <v>0.59420038477725012</v>
       </c>
@@ -5443,7 +5443,7 @@
         <f t="shared" si="42"/>
         <v>170.00000000000011</v>
       </c>
-      <c r="P73" s="38">
+      <c r="P73" s="32">
         <f t="shared" si="44"/>
         <v>0.59062514941429611</v>
       </c>
@@ -5510,7 +5510,7 @@
         <f t="shared" si="42"/>
         <v>172.50000000000014</v>
       </c>
-      <c r="P74" s="38">
+      <c r="P74" s="32">
         <f t="shared" si="44"/>
         <v>0.58709197314479233</v>
       </c>
@@ -5577,7 +5577,7 @@
         <f t="shared" si="42"/>
         <v>175.00000000000014</v>
       </c>
-      <c r="P75" s="38">
+      <c r="P75" s="32">
         <f t="shared" si="44"/>
         <v>0.583600118133491</v>
       </c>
@@ -5644,7 +5644,7 @@
         <f t="shared" si="42"/>
         <v>177.50000000000014</v>
       </c>
-      <c r="P76" s="38">
+      <c r="P76" s="32">
         <f t="shared" si="44"/>
         <v>0.58014886370309482</v>
       </c>
@@ -5711,7 +5711,7 @@
         <f t="shared" si="42"/>
         <v>180.00000000000014</v>
       </c>
-      <c r="P77" s="38">
+      <c r="P77" s="32">
         <f t="shared" si="44"/>
         <v>0.57673750583839334</v>
       </c>
@@ -5778,7 +5778,7 @@
         <f t="shared" si="42"/>
         <v>182.50000000000017</v>
       </c>
-      <c r="P78" s="38">
+      <c r="P78" s="32">
         <f t="shared" si="44"/>
         <v>0.573365356707494</v>
       </c>
@@ -5845,7 +5845,7 @@
         <f t="shared" si="42"/>
         <v>185.00000000000017</v>
       </c>
-      <c r="P79" s="38">
+      <c r="P79" s="32">
         <f t="shared" si="44"/>
         <v>0.57003174419946889</v>
       </c>
@@ -5912,7 +5912,7 @@
         <f t="shared" si="42"/>
         <v>187.50000000000014</v>
       </c>
-      <c r="P80" s="38">
+      <c r="P80" s="32">
         <f t="shared" si="44"/>
         <v>0.56673601147776187</v>
       </c>
@@ -5979,7 +5979,7 @@
         <f t="shared" si="42"/>
         <v>190.0000000000002</v>
       </c>
-      <c r="P81" s="38">
+      <c r="P81" s="32">
         <f t="shared" si="44"/>
         <v>0.56347751654873302</v>
       </c>
@@ -6046,7 +6046,7 @@
         <f t="shared" si="42"/>
         <v>192.50000000000017</v>
       </c>
-      <c r="P82" s="38">
+      <c r="P82" s="32">
         <f t="shared" si="44"/>
         <v>0.56025563184474825</v>
       </c>
@@ -6113,7 +6113,7 @@
         <f t="shared" si="42"/>
         <v>195.0000000000002</v>
       </c>
-      <c r="P83" s="38">
+      <c r="P83" s="32">
         <f t="shared" si="44"/>
         <v>0.55706974382123919</v>
       </c>
@@ -6180,7 +6180,7 @@
         <f t="shared" si="42"/>
         <v>197.50000000000017</v>
       </c>
-      <c r="P84" s="38">
+      <c r="P84" s="32">
         <f t="shared" si="44"/>
         <v>0.55391925256719599</v>
       </c>
@@ -6247,7 +6247,7 @@
         <f t="shared" si="42"/>
         <v>200.00000000000017</v>
       </c>
-      <c r="P85" s="38">
+      <c r="P85" s="32">
         <f t="shared" si="44"/>
         <v>0.5508035714285715</v>
       </c>
@@ -6314,7 +6314,7 @@
         <f t="shared" si="42"/>
         <v>202.50000000000014</v>
       </c>
-      <c r="P86" s="38">
+      <c r="P86" s="32">
         <f t="shared" si="44"/>
         <v>0.54772212664409792</v>
       </c>
@@ -6381,7 +6381,7 @@
         <f t="shared" si="42"/>
         <v>205.00000000000014</v>
       </c>
-      <c r="P87" s="38">
+      <c r="P87" s="32">
         <f t="shared" si="44"/>
         <v>0.54467435699304567</v>
       </c>
@@ -6448,7 +6448,7 @@
         <f t="shared" si="42"/>
         <v>207.50000000000011</v>
       </c>
-      <c r="P88" s="38">
+      <c r="P88" s="32">
         <f t="shared" si="44"/>
         <v>0.54165971345446562</v>
       </c>
@@ -6515,7 +6515,7 @@
         <f t="shared" si="42"/>
         <v>210.00000000000011</v>
       </c>
-      <c r="P89" s="38">
+      <c r="P89" s="32">
         <f t="shared" si="44"/>
         <v>0.5386776588774842</v>
       </c>
@@ -6582,7 +6582,7 @@
         <f t="shared" si="42"/>
         <v>212.50000000000011</v>
       </c>
-      <c r="P90" s="38">
+      <c r="P90" s="32">
         <f t="shared" si="44"/>
         <v>0.53572766766223201</v>
       </c>
@@ -6649,7 +6649,7 @@
         <f t="shared" si="42"/>
         <v>215.00000000000009</v>
       </c>
-      <c r="P91" s="38">
+      <c r="P91" s="32">
         <f t="shared" si="44"/>
         <v>0.53280922545100995</v>
       </c>
@@ -6716,7 +6716,7 @@
         <f t="shared" si="42"/>
         <v>217.50000000000009</v>
       </c>
-      <c r="P92" s="38">
+      <c r="P92" s="32">
         <f t="shared" si="44"/>
         <v>0.52992182882931282</v>
       </c>
@@ -6783,7 +6783,7 @@
         <f t="shared" si="42"/>
         <v>220.00000000000006</v>
       </c>
-      <c r="P93" s="38">
+      <c r="P93" s="32">
         <f t="shared" si="44"/>
         <v>0.52706498503634058</v>
       </c>
@@ -6850,7 +6850,7 @@
         <f t="shared" si="42"/>
         <v>222.50000000000006</v>
       </c>
-      <c r="P94" s="38">
+      <c r="P94" s="32">
         <f t="shared" si="44"/>
         <v>0.52423821168465268</v>
       </c>
@@ -6917,7 +6917,7 @@
         <f t="shared" si="42"/>
         <v>225.00000000000006</v>
       </c>
-      <c r="P95" s="38">
+      <c r="P95" s="32">
         <f t="shared" si="44"/>
         <v>0.5214410364886306</v>
       </c>
@@ -6984,7 +6984,7 @@
         <f t="shared" si="42"/>
         <v>227.50000000000003</v>
       </c>
-      <c r="P96" s="38">
+      <c r="P96" s="32">
         <f t="shared" si="44"/>
         <v>0.51867299700142055</v>
       </c>
@@ -7051,7 +7051,7 @@
         <f t="shared" si="42"/>
         <v>230</v>
       </c>
-      <c r="P97" s="38">
+      <c r="P97" s="32">
         <f t="shared" si="44"/>
         <v>0.51593364036005884</v>
       </c>
@@ -7118,7 +7118,7 @@
         <f t="shared" si="42"/>
         <v>232.49999999999997</v>
       </c>
-      <c r="P98" s="38">
+      <c r="P98" s="32">
         <f t="shared" si="44"/>
         <v>0.51322252303847593</v>
       </c>
@@ -7185,7 +7185,7 @@
         <f t="shared" si="42"/>
         <v>234.99999999999994</v>
       </c>
-      <c r="P99" s="38">
+      <c r="P99" s="32">
         <f t="shared" si="44"/>
         <v>0.51053921060810137</v>
       </c>
@@ -7252,7 +7252,7 @@
         <f t="shared" si="42"/>
         <v>237.49999999999994</v>
       </c>
-      <c r="P100" s="38">
+      <c r="P100" s="32">
         <f t="shared" si="44"/>
         <v>0.50788327750579776</v>
       </c>
@@ -7319,7 +7319,7 @@
         <f t="shared" ref="O101:O105" si="53">N101*G101</f>
         <v>239.99999999999994</v>
       </c>
-      <c r="P101" s="38">
+      <c r="P101" s="32">
         <f t="shared" si="44"/>
         <v>0.50525430680885997</v>
       </c>
@@ -7386,7 +7386,7 @@
         <f t="shared" si="53"/>
         <v>242.49999999999991</v>
       </c>
-      <c r="P102" s="38">
+      <c r="P102" s="32">
         <f t="shared" si="44"/>
         <v>0.50265189001683452</v>
       </c>
@@ -7453,7 +7453,7 @@
         <f t="shared" si="53"/>
         <v>244.99999999999989</v>
       </c>
-      <c r="P103" s="38">
+      <c r="P103" s="32">
         <f t="shared" si="44"/>
         <v>0.50007562683991502</v>
       </c>
@@ -7520,7 +7520,7 @@
         <f t="shared" si="53"/>
         <v>247.49999999999989</v>
       </c>
-      <c r="P104" s="38">
+      <c r="P104" s="32">
         <f t="shared" si="44"/>
         <v>0.49752512499368762</v>
       </c>
@@ -7587,7 +7587,7 @@
         <f t="shared" si="53"/>
         <v>249.99999999999989</v>
       </c>
-      <c r="P105" s="39">
+      <c r="P105" s="33">
         <f t="shared" si="44"/>
         <v>0.49500000000000033</v>
       </c>

</xml_diff>